<commit_message>
[WIP] adding a parameter in column format to the spreadsheet and toy case study
</commit_message>
<xml_diff>
--- a/pareto/case_studies/toy_case_study.xlsx
+++ b/pareto/case_studies/toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091E7FB3-DD8A-46C0-BABA-82724DD66482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFBD34E-9C5E-48F9-BD03-9BC360973386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="2" activeTab="8" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="3" activeTab="9" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId7"/>
     <sheet name="FlowbackRates" sheetId="12" r:id="rId8"/>
     <sheet name="ProductionRates" sheetId="34" r:id="rId9"/>
+    <sheet name="InitialDisposalCapacity" sheetId="36" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="91">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -303,6 +304,9 @@
   </si>
   <si>
     <t>List of all Production Tank Identifiers [-]</t>
+  </si>
+  <si>
+    <t>Table of Initial Disposal Capacity  [bbl/day]</t>
   </si>
 </sst>
 </file>
@@ -1632,6 +1636,74 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AFB15B-B1C8-461A-BF7D-18135C4BCB65}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="22">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="22">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="22">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
   <dimension ref="A1:R16"/>
@@ -4725,7 +4797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B919BA92-5244-487C-A2DC-E363C6C267C1}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Extending get_data to read parameters with multiple indices in column format. Updating toy case study. Updating gitignore to ignore temporary excel files
</commit_message>
<xml_diff>
--- a/pareto/case_studies/toy_case_study.xlsx
+++ b/pareto/case_studies/toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFBD34E-9C5E-48F9-BD03-9BC360973386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F2FFB8-27DC-4333-ACA0-2C8A9443A87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="3" activeTab="9" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="5" activeTab="10" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="FlowbackRates" sheetId="12" r:id="rId8"/>
     <sheet name="ProductionRates" sheetId="34" r:id="rId9"/>
     <sheet name="InitialDisposalCapacity" sheetId="36" r:id="rId10"/>
+    <sheet name="TwoIndexColumnParam" sheetId="37" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -1640,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AFB15B-B1C8-461A-BF7D-18135C4BCB65}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -1695,6 +1696,91 @@
         <v>28</v>
       </c>
       <c r="B7" s="22">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8364E144-4CD2-44C5-A585-25BE71A80703}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="22">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="22">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="22">
         <v>5000</v>
       </c>
     </row>
@@ -2191,7 +2277,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -3399,7 +3485,7 @@
   <dimension ref="A1:BA17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
adding method to check data consistency
</commit_message>
<xml_diff>
--- a/pareto/case_studies/toy_case_study.xlsx
+++ b/pareto/case_studies/toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F2FFB8-27DC-4333-ACA0-2C8A9443A87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C398DE0-B5E2-4D85-A58C-268CB4A366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="5" activeTab="10" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="2" activeTab="8" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1710,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8364E144-4CD2-44C5-A585-25BE71A80703}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -4883,8 +4883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B919BA92-5244-487C-A2DC-E363C6C267C1}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
adding od_matrix method to obtain data for drive times and drive distances between locations
</commit_message>
<xml_diff>
--- a/pareto/case_studies/toy_case_study.xlsx
+++ b/pareto/case_studies/toy_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C398DE0-B5E2-4D85-A58C-268CB4A366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95A7432-E439-4718-AF9E-8F0A7CD1F91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="2" activeTab="8" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="4" activeTab="6" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="SWDSites" sheetId="4" r:id="rId4"/>
     <sheet name="ProductionTanks" sheetId="35" r:id="rId5"/>
     <sheet name="DriveTimes" sheetId="7" r:id="rId6"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId7"/>
-    <sheet name="FlowbackRates" sheetId="12" r:id="rId8"/>
-    <sheet name="ProductionRates" sheetId="34" r:id="rId9"/>
-    <sheet name="InitialDisposalCapacity" sheetId="36" r:id="rId10"/>
-    <sheet name="TwoIndexColumnParam" sheetId="37" r:id="rId11"/>
+    <sheet name="Coordinates" sheetId="38" r:id="rId7"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId8"/>
+    <sheet name="FlowbackRates" sheetId="12" r:id="rId9"/>
+    <sheet name="ProductionRates" sheetId="34" r:id="rId10"/>
+    <sheet name="InitialDisposalCapacity" sheetId="36" r:id="rId11"/>
+    <sheet name="TwoIndexColumnParam" sheetId="37" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="94">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -308,12 +309,24 @@
   </si>
   <si>
     <t>Table of Initial Disposal Capacity  [bbl/day]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinates </t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -716,6 +729,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1638,11 +1652,380 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B919BA92-5244-487C-A2DC-E363C6C267C1}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="2" width="9.26171875" style="18"/>
+    <col min="3" max="16384" width="9.26171875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <v>3</v>
+      </c>
+      <c r="F2" s="16">
+        <v>4</v>
+      </c>
+      <c r="G2" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1058</v>
+      </c>
+      <c r="D3" s="42">
+        <v>1029</v>
+      </c>
+      <c r="E3" s="42">
+        <v>999</v>
+      </c>
+      <c r="F3" s="42">
+        <v>998</v>
+      </c>
+      <c r="G3" s="20">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="42">
+        <v>1058</v>
+      </c>
+      <c r="D4" s="42">
+        <v>1029</v>
+      </c>
+      <c r="E4" s="42">
+        <v>999</v>
+      </c>
+      <c r="F4" s="42">
+        <v>998</v>
+      </c>
+      <c r="G4" s="20">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="42">
+        <v>466</v>
+      </c>
+      <c r="D5" s="42">
+        <v>460</v>
+      </c>
+      <c r="E5" s="42">
+        <v>458</v>
+      </c>
+      <c r="F5" s="42">
+        <v>457</v>
+      </c>
+      <c r="G5" s="20">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="42">
+        <v>466</v>
+      </c>
+      <c r="D6" s="42">
+        <v>460</v>
+      </c>
+      <c r="E6" s="42">
+        <v>458</v>
+      </c>
+      <c r="F6" s="42">
+        <v>457</v>
+      </c>
+      <c r="G6" s="20">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="42">
+        <v>466</v>
+      </c>
+      <c r="D7" s="42">
+        <v>460</v>
+      </c>
+      <c r="E7" s="42">
+        <v>458</v>
+      </c>
+      <c r="F7" s="42">
+        <v>457</v>
+      </c>
+      <c r="G7" s="20">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="42">
+        <v>200</v>
+      </c>
+      <c r="D8" s="42">
+        <v>199</v>
+      </c>
+      <c r="E8" s="42">
+        <v>198</v>
+      </c>
+      <c r="F8" s="42">
+        <v>196</v>
+      </c>
+      <c r="G8" s="20">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="42">
+        <v>200</v>
+      </c>
+      <c r="D9" s="42">
+        <v>199</v>
+      </c>
+      <c r="E9" s="42">
+        <v>198</v>
+      </c>
+      <c r="F9" s="42">
+        <v>196</v>
+      </c>
+      <c r="G9" s="20">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="42">
+        <v>200</v>
+      </c>
+      <c r="D10" s="42">
+        <v>199</v>
+      </c>
+      <c r="E10" s="42">
+        <v>198</v>
+      </c>
+      <c r="F10" s="42">
+        <v>196</v>
+      </c>
+      <c r="G10" s="20">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="42">
+        <v>200</v>
+      </c>
+      <c r="D11" s="42">
+        <v>199</v>
+      </c>
+      <c r="E11" s="42">
+        <v>198</v>
+      </c>
+      <c r="F11" s="42">
+        <v>196</v>
+      </c>
+      <c r="G11" s="20">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="42">
+        <v>331</v>
+      </c>
+      <c r="D12" s="42">
+        <v>330</v>
+      </c>
+      <c r="E12" s="42">
+        <v>330</v>
+      </c>
+      <c r="F12" s="42">
+        <v>329</v>
+      </c>
+      <c r="G12" s="20">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="42">
+        <v>331</v>
+      </c>
+      <c r="D13" s="42">
+        <v>330</v>
+      </c>
+      <c r="E13" s="42">
+        <v>330</v>
+      </c>
+      <c r="F13" s="42">
+        <v>329</v>
+      </c>
+      <c r="G13" s="20">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="42">
+        <v>331</v>
+      </c>
+      <c r="D14" s="42">
+        <v>330</v>
+      </c>
+      <c r="E14" s="42">
+        <v>330</v>
+      </c>
+      <c r="F14" s="42">
+        <v>329</v>
+      </c>
+      <c r="G14" s="20">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="42">
+        <v>895</v>
+      </c>
+      <c r="D15" s="42">
+        <v>888</v>
+      </c>
+      <c r="E15" s="42">
+        <v>887</v>
+      </c>
+      <c r="F15" s="42">
+        <v>885</v>
+      </c>
+      <c r="G15" s="20">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="21">
+        <v>895</v>
+      </c>
+      <c r="D16" s="21">
+        <v>888</v>
+      </c>
+      <c r="E16" s="21">
+        <v>887</v>
+      </c>
+      <c r="F16" s="21">
+        <v>885</v>
+      </c>
+      <c r="G16" s="22">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" s="47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AFB15B-B1C8-461A-BF7D-18135C4BCB65}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -1706,7 +2089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8364E144-4CD2-44C5-A585-25BE71A80703}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2574,7 +2957,7 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="A3" sqref="A3:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -3481,6 +3864,300 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BF3884-09AC-4C78-8EAF-AA69EB452744}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>47.604399999999998</v>
+      </c>
+      <c r="C3">
+        <v>-122.33450000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="49">
+        <v>47.678551400158099</v>
+      </c>
+      <c r="C4" s="49">
+        <v>-122.38514810411333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="49">
+        <v>47.671605016754775</v>
+      </c>
+      <c r="C5" s="49">
+        <v>-122.31941699831951</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="49">
+        <v>47.51373173275276</v>
+      </c>
+      <c r="C6" s="49">
+        <v>-122.37256636119979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="49">
+        <v>47.598210949478798</v>
+      </c>
+      <c r="C7" s="49">
+        <v>-122.30833430642372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="49">
+        <v>47.545013073705562</v>
+      </c>
+      <c r="C8" s="49">
+        <v>-122.27578180785954</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="49">
+        <v>47.531980739789113</v>
+      </c>
+      <c r="C9" s="49">
+        <v>-122.25392487570376</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="49">
+        <v>47.56473303789118</v>
+      </c>
+      <c r="C10" s="49">
+        <v>-122.23615203748196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="49">
+        <v>47.529792632940953</v>
+      </c>
+      <c r="C11" s="49">
+        <v>-122.38490267916536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="49">
+        <v>47.631685383062539</v>
+      </c>
+      <c r="C12" s="49">
+        <v>-122.43178036972577</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="49">
+        <v>47.662203296426647</v>
+      </c>
+      <c r="C13" s="49">
+        <v>-122.3748467760494</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="49">
+        <v>47.650576946946856</v>
+      </c>
+      <c r="C14" s="49">
+        <v>-122.33832847843796</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="49">
+        <v>47.655834380297506</v>
+      </c>
+      <c r="C15" s="49">
+        <v>-122.24953147273567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="49">
+        <v>47.680787091717839</v>
+      </c>
+      <c r="C16" s="49">
+        <v>-122.27548462416144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="49">
+        <v>47.53282219470006</v>
+      </c>
+      <c r="C17" s="49">
+        <v>-122.41679135415569</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="49">
+        <v>47.623906510821413</v>
+      </c>
+      <c r="C18" s="49">
+        <v>-122.36685609717435</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="49">
+        <v>47.544942555956496</v>
+      </c>
+      <c r="C19" s="49">
+        <v>-122.39902392056128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="49">
+        <v>47.546281351253072</v>
+      </c>
+      <c r="C20" s="49">
+        <v>-122.2875801822827</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="49">
+        <v>47.599229667613891</v>
+      </c>
+      <c r="C21" s="49">
+        <v>-122.2901468966058</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="49">
+        <v>47.632141396558332</v>
+      </c>
+      <c r="C22" s="49">
+        <v>-122.29739693081503</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="49">
+        <v>47.606697845554585</v>
+      </c>
+      <c r="C23" s="49">
+        <v>-122.39872536852423</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="49">
+        <v>47.616415359392079</v>
+      </c>
+      <c r="C24" s="49">
+        <v>-122.26887716808142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="49">
+        <v>47.600371580577168</v>
+      </c>
+      <c r="C25" s="49">
+        <v>-122.27286360239516</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="49">
+        <v>47.534616037389881</v>
+      </c>
+      <c r="C26" s="49">
+        <v>-122.27032458981431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:BA17"/>
   <sheetViews>
@@ -4146,7 +4823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
   <dimension ref="A1:BA22"/>
   <sheetViews>
@@ -4877,373 +5554,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B919BA92-5244-487C-A2DC-E363C6C267C1}">
-  <dimension ref="A1:G21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="2" width="9.26171875" style="18"/>
-    <col min="3" max="16384" width="9.26171875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="15"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="16">
-        <v>2</v>
-      </c>
-      <c r="E2" s="16">
-        <v>3</v>
-      </c>
-      <c r="F2" s="16">
-        <v>4</v>
-      </c>
-      <c r="G2" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1058</v>
-      </c>
-      <c r="D3" s="42">
-        <v>1029</v>
-      </c>
-      <c r="E3" s="42">
-        <v>999</v>
-      </c>
-      <c r="F3" s="42">
-        <v>998</v>
-      </c>
-      <c r="G3" s="20">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="42">
-        <v>1058</v>
-      </c>
-      <c r="D4" s="42">
-        <v>1029</v>
-      </c>
-      <c r="E4" s="42">
-        <v>999</v>
-      </c>
-      <c r="F4" s="42">
-        <v>998</v>
-      </c>
-      <c r="G4" s="20">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="42">
-        <v>466</v>
-      </c>
-      <c r="D5" s="42">
-        <v>460</v>
-      </c>
-      <c r="E5" s="42">
-        <v>458</v>
-      </c>
-      <c r="F5" s="42">
-        <v>457</v>
-      </c>
-      <c r="G5" s="20">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="42">
-        <v>466</v>
-      </c>
-      <c r="D6" s="42">
-        <v>460</v>
-      </c>
-      <c r="E6" s="42">
-        <v>458</v>
-      </c>
-      <c r="F6" s="42">
-        <v>457</v>
-      </c>
-      <c r="G6" s="20">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="42">
-        <v>466</v>
-      </c>
-      <c r="D7" s="42">
-        <v>460</v>
-      </c>
-      <c r="E7" s="42">
-        <v>458</v>
-      </c>
-      <c r="F7" s="42">
-        <v>457</v>
-      </c>
-      <c r="G7" s="20">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="42">
-        <v>200</v>
-      </c>
-      <c r="D8" s="42">
-        <v>199</v>
-      </c>
-      <c r="E8" s="42">
-        <v>198</v>
-      </c>
-      <c r="F8" s="42">
-        <v>196</v>
-      </c>
-      <c r="G8" s="20">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="42">
-        <v>200</v>
-      </c>
-      <c r="D9" s="42">
-        <v>199</v>
-      </c>
-      <c r="E9" s="42">
-        <v>198</v>
-      </c>
-      <c r="F9" s="42">
-        <v>196</v>
-      </c>
-      <c r="G9" s="20">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="42">
-        <v>200</v>
-      </c>
-      <c r="D10" s="42">
-        <v>199</v>
-      </c>
-      <c r="E10" s="42">
-        <v>198</v>
-      </c>
-      <c r="F10" s="42">
-        <v>196</v>
-      </c>
-      <c r="G10" s="20">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="42">
-        <v>200</v>
-      </c>
-      <c r="D11" s="42">
-        <v>199</v>
-      </c>
-      <c r="E11" s="42">
-        <v>198</v>
-      </c>
-      <c r="F11" s="42">
-        <v>196</v>
-      </c>
-      <c r="G11" s="20">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="42">
-        <v>331</v>
-      </c>
-      <c r="D12" s="42">
-        <v>330</v>
-      </c>
-      <c r="E12" s="42">
-        <v>330</v>
-      </c>
-      <c r="F12" s="42">
-        <v>329</v>
-      </c>
-      <c r="G12" s="20">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="42">
-        <v>331</v>
-      </c>
-      <c r="D13" s="42">
-        <v>330</v>
-      </c>
-      <c r="E13" s="42">
-        <v>330</v>
-      </c>
-      <c r="F13" s="42">
-        <v>329</v>
-      </c>
-      <c r="G13" s="20">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="42">
-        <v>331</v>
-      </c>
-      <c r="D14" s="42">
-        <v>330</v>
-      </c>
-      <c r="E14" s="42">
-        <v>330</v>
-      </c>
-      <c r="F14" s="42">
-        <v>329</v>
-      </c>
-      <c r="G14" s="20">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="42">
-        <v>895</v>
-      </c>
-      <c r="D15" s="42">
-        <v>888</v>
-      </c>
-      <c r="E15" s="42">
-        <v>887</v>
-      </c>
-      <c r="F15" s="42">
-        <v>885</v>
-      </c>
-      <c r="G15" s="20">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="21">
-        <v>895</v>
-      </c>
-      <c r="D16" s="21">
-        <v>888</v>
-      </c>
-      <c r="E16" s="21">
-        <v>887</v>
-      </c>
-      <c r="F16" s="21">
-        <v>885</v>
-      </c>
-      <c r="G16" s="22">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="G21" s="47"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changing data request from GET to POST. Reformatting get_data module to comply with pylint
</commit_message>
<xml_diff>
--- a/pareto/case_studies/toy_case_study.xlsx
+++ b/pareto/case_studies/toy_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95A7432-E439-4718-AF9E-8F0A7CD1F91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02562E84-8559-4CE0-AC85-5D3F92ACE13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="4" activeTab="6" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -325,7 +325,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -729,7 +729,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3868,10 +3868,14 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="16.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
@@ -3892,10 +3896,10 @@
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="49">
         <v>47.604399999999998</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="49">
         <v>-122.33450000000001</v>
       </c>
     </row>

</xml_diff>